<commit_message>
TODO: Fix calendar range for student and teacher invoice
</commit_message>
<xml_diff>
--- a/gui/template/Student Base Template.xlsx
+++ b/gui/template/Student Base Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruele\PycharmProjects\RueLee\BostonEdu_Invoice_2023\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruele\PycharmProjects\RueLee\Boston Education\bosvoiceton-gui\gui\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6CFEF2-9200-49AF-AA93-1DEEAF470A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5532D249-FAF5-4157-9001-AD058651B384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="root" sheetId="2" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>Boston Education Institute</t>
   </si>
   <si>
-    <t>4311 Wilshire Blvd., #530A</t>
-  </si>
-  <si>
     <t>Los Angeles, CA 90010</t>
   </si>
   <si>
@@ -105,10 +102,34 @@
     <t>Invoice#:</t>
   </si>
   <si>
-    <t>Pay to the order: Boston Education</t>
-  </si>
-  <si>
     <t>Balance/Credit from last invoice:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pay to the order</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Boston Education</t>
+    </r>
+  </si>
+  <si>
+    <t>4211 Wilshire Blvd., Suite 136</t>
   </si>
 </sst>
 </file>
@@ -119,7 +140,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +230,22 @@
     </font>
     <font>
       <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -506,9 +543,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -574,6 +608,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -941,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,12 +1000,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="32.25" x14ac:dyDescent="0.55000000000000004">
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="8"/>
+      <c r="F1" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" s="11"/>
-      <c r="F1" s="13" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -972,249 +1015,252 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="14"/>
+        <v>5</v>
+      </c>
+      <c r="G3" s="11"/>
     </row>
     <row r="4" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="15"/>
+        <v>21</v>
+      </c>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="15"/>
+        <v>1</v>
+      </c>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="2:7" ht="21" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="15"/>
+        <v>6</v>
+      </c>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" spans="2:7" ht="21" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="16"/>
+      <c r="G7" s="13"/>
     </row>
     <row r="8" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="15"/>
+        <v>4</v>
+      </c>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7"/>
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="4"/>
     </row>
     <row r="11" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="5"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="34"/>
     </row>
     <row r="12" spans="2:7" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="D13" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="E13" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="F13" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="G13" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="24" t="s">
+    </row>
+    <row r="14" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B14" s="22"/>
+      <c r="C14" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="25"/>
+    </row>
+    <row r="15" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B15" s="14"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="16"/>
+    </row>
+    <row r="16" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B16" s="17"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="16"/>
+    </row>
+    <row r="17" spans="2:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16"/>
+    </row>
+    <row r="18" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="19" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B19" s="17"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="16"/>
+    </row>
+    <row r="20" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B20" s="17"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="16"/>
+    </row>
+    <row r="21" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B21" s="17"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16"/>
+    </row>
+    <row r="22" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B22" s="17"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="16"/>
+    </row>
+    <row r="23" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B23" s="17"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="16"/>
+    </row>
+    <row r="24" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B24" s="17"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="16"/>
+    </row>
+    <row r="25" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B25" s="17"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="16"/>
+    </row>
+    <row r="26" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B26" s="17"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="16"/>
+    </row>
+    <row r="27" spans="2:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="29"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="31"/>
+    </row>
+    <row r="28" spans="2:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B14" s="25"/>
-      <c r="C14" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="28"/>
-    </row>
-    <row r="15" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="19"/>
-    </row>
-    <row r="16" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B16" s="20"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="19"/>
-    </row>
-    <row r="17" spans="2:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="19"/>
-    </row>
-    <row r="18" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="19"/>
-    </row>
-    <row r="19" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B19" s="20"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="19"/>
-    </row>
-    <row r="20" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B20" s="20"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="19"/>
-    </row>
-    <row r="21" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B21" s="20"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="19"/>
-    </row>
-    <row r="22" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B22" s="20"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="19"/>
-    </row>
-    <row r="23" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B23" s="20"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="19"/>
-    </row>
-    <row r="24" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B24" s="20"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="19"/>
-    </row>
-    <row r="25" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B25" s="20"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="19"/>
-    </row>
-    <row r="26" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B26" s="20"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="19"/>
-    </row>
-    <row r="27" spans="2:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="32"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="34"/>
-    </row>
-    <row r="28" spans="2:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G28" s="21">
+      <c r="G28" s="18">
         <f>SUM(G14:G27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="10" t="s">
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B11:G11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Updated Excel sheet and database
</commit_message>
<xml_diff>
--- a/gui/template/Student Base Template.xlsx
+++ b/gui/template/Student Base Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruele\PycharmProjects\RueLee\Boston Education\bosvoiceton-gui\gui\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5532D249-FAF5-4157-9001-AD058651B384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951FF907-0732-45F7-BC44-A69BE796F273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,6 +105,9 @@
     <t>Balance/Credit from last invoice:</t>
   </si>
   <si>
+    <t>4211 Wilshire Blvd., Suite 136</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -125,11 +128,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: Boston Education</t>
+      <t>: Boston Education | (Venmo: @bostonedu; Zelle - 213-500-0101)</t>
     </r>
-  </si>
-  <si>
-    <t>4211 Wilshire Blvd., Suite 136</t>
   </si>
 </sst>
 </file>
@@ -985,7 +985,7 @@
   <dimension ref="B1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,7 +1021,7 @@
     </row>
     <row r="4" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>21</v>
@@ -1069,7 +1069,7 @@
     </row>
     <row r="11" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="32" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>

</xml_diff>